<commit_message>
complete every things except two tabs
</commit_message>
<xml_diff>
--- a/FactoryMonitoringSystem/Users.xlsx
+++ b/FactoryMonitoringSystem/Users.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Programming\MATLAB\FactoryMonitoringSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF2FC09-ECCA-4A42-A2BB-63CC6D3F017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A99D410-5605-4EF5-BC6A-099955096807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>UserID</t>
   </si>
@@ -33,61 +28,47 @@
     <t>Username</t>
   </si>
   <si>
+    <t>admin_user</t>
+  </si>
+  <si>
+    <t>operator_user</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>ali rezaii</t>
-  </si>
-  <si>
-    <t>sara mohammadi</t>
-  </si>
-  <si>
-    <t>hossein karimi</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>operator1</t>
-  </si>
-  <si>
-    <t>operator2</t>
-  </si>
-  <si>
-    <t>operator</t>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>op456</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>33333a</t>
-  </si>
-  <si>
-    <t>11111a</t>
-  </si>
-  <si>
-    <t>12345a</t>
+    <t>Admin Name</t>
+  </si>
+  <si>
+    <t>Operator Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,11 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,39 +121,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,9 +186,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -243,6 +238,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -304,13 +316,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -319,6 +324,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -383,11 +395,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,88 +427,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="5" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>